<commit_message>
last test and twist test
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/jvt122_ic_ac_uk/Documents/Project/Experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/jvt122_ic_ac_uk/Documents/Project/Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="515" documentId="8_{72CA102F-2BD9-4E63-A6F7-B5D089D94F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D503213-60FA-4431-959D-A0A186CB8C07}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="8_{72CA102F-2BD9-4E63-A6F7-B5D089D94F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F351A94C-2107-447B-8A52-DAB38D784DBC}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{A6EA9410-D058-4DEA-B47E-813B62B2F81E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A6EA9410-D058-4DEA-B47E-813B62B2F81E}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnarie" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
   <si>
     <t>M</t>
   </si>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6987DE-497F-4621-BC37-A41ECCE5E82B}">
   <dimension ref="A1:AI42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,7 +531,7 @@
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -562,8 +562,11 @@
       <c r="K1">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -597,8 +600,11 @@
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -632,8 +638,11 @@
       <c r="K3" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -667,8 +676,11 @@
       <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -702,8 +714,11 @@
       <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -737,8 +752,11 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -772,8 +790,11 @@
       <c r="K7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -807,8 +828,11 @@
       <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -842,8 +866,11 @@
       <c r="K9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -877,8 +904,11 @@
       <c r="K10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -912,8 +942,11 @@
       <c r="K11" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -947,8 +980,11 @@
       <c r="K12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -982,8 +1018,11 @@
       <c r="K13" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1017,8 +1056,11 @@
       <c r="K14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1052,8 +1094,11 @@
       <c r="K15" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1087,8 +1132,11 @@
       <c r="K16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1122,8 +1170,11 @@
       <c r="K17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1157,8 +1208,11 @@
       <c r="K18" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1192,8 +1246,11 @@
       <c r="K19" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1227,8 +1284,11 @@
       <c r="K20" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1262,8 +1322,11 @@
       <c r="K21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1297,8 +1360,11 @@
       <c r="K22" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1332,8 +1398,11 @@
       <c r="K23" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1367,8 +1436,11 @@
       <c r="K24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1402,8 +1474,11 @@
       <c r="K25" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1437,8 +1512,11 @@
       <c r="K26" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1472,8 +1550,11 @@
       <c r="K27" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1507,8 +1588,11 @@
       <c r="K28" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1542,8 +1626,11 @@
       <c r="K29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1576,6 +1663,9 @@
       </c>
       <c r="K30" s="1">
         <v>4</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:35" x14ac:dyDescent="0.3">
@@ -1898,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04486DC4-DB2B-4AAB-9BF5-EEEB645F475F}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1909,7 +1999,7 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -1940,8 +2030,11 @@
       <c r="K1">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1975,8 +2068,11 @@
       <c r="K2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2010,8 +2106,11 @@
       <c r="K3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2045,8 +2144,11 @@
       <c r="K4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2080,8 +2182,11 @@
       <c r="K5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2115,8 +2220,11 @@
       <c r="K6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2150,8 +2258,11 @@
       <c r="K7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2185,8 +2296,11 @@
       <c r="K8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2220,8 +2334,11 @@
       <c r="K9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2255,8 +2372,11 @@
       <c r="K10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2289,6 +2409,9 @@
       </c>
       <c r="K11">
         <v>11</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>